<commit_message>
RawData to ParsedRecord converting implementation updated
</commit_message>
<xml_diff>
--- a/ms-service/src/test/resources/test_restriction_070116.xlsx
+++ b/ms-service/src/test/resources/test_restriction_070116.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>test_asset_allocation</t>
+  </si>
+  <si>
+    <t>test_book_2</t>
+  </si>
+  <si>
+    <t>test_location_2</t>
+  </si>
+  <si>
+    <t>test_subsidiary_2</t>
+  </si>
+  <si>
+    <t>test_organisation_2</t>
+  </si>
+  <si>
+    <t>test_risk_class_2</t>
+  </si>
+  <si>
+    <t>test_var_hierarchy_2</t>
+  </si>
+  <si>
+    <t>var_facet_2</t>
+  </si>
+  <si>
+    <t>test_asset_allocation_2</t>
   </si>
 </sst>
 </file>
@@ -405,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,6 +520,41 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>